<commit_message>
pic of street in morocco
</commit_message>
<xml_diff>
--- a/work/dbg/docs/Budget.xlsx
+++ b/work/dbg/docs/Budget.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sandbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sandbox\code\work\dbg\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5B1B19-B66C-499C-8778-83704ED8A730}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCB5455-F106-4041-B36E-5E90E246D5F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7079818F-CE79-4E2B-8877-60450D0B80A7}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -106,7 +106,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -257,21 +257,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -590,7 +590,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>